<commit_message>
Added Solar and GHL Changes
</commit_message>
<xml_diff>
--- a/conversation_templates.xlsx
+++ b/conversation_templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\InteractiveAvatarNextJSDemo\AI_convo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8DAF0A85-271D-4B49-9613-CE0D74A94A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51588B2-17A0-4412-8896-2C75E09B43E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{49CED437-DC61-418D-B761-02FA15BBEAEE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
   <si>
     <t>Role</t>
   </si>
@@ -60,15 +60,9 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Taking you to https://squidgy.ai/</t>
-  </si>
-  <si>
     <t>Hi! I'm Squidgy and I'm here to help you win back time and make more money. Think of me as like a consultant who can instantly build you a solution to a bunch of your problems.To get started, could you tell me your website?</t>
   </si>
   <si>
-    <t>BusinessManager</t>
-  </si>
-  <si>
     <t>Good to konw. That's not cheap, but I like that it's low risk. So there are ZERO setup or monthly fees?</t>
   </si>
   <si>
@@ -94,9 +88,6 @@
   </si>
   <si>
     <t>Yep, I'm good with that</t>
-  </si>
-  <si>
-    <t>DomainExpert</t>
   </si>
   <si>
     <t>Fab. Just to let you know what will happen next. I'll need to ask you about X questions. This should take around 30 minutes. One thing you might need to think about first is your pricing structure - I need this so I can provide accurate cost estimates in the proposals I build for your clients. However I can build your demo using market average pricing, if you'd just like to get your demo up and running quickly. Would you like to go ahead now? Or would you prefer to go away and prepare? I can remind you later, if so.</t>
@@ -232,10 +223,10 @@
     <t>{Domain Specific}</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>Clients probable response</t>
+  </si>
+  <si>
+    <t>SocialMediaManager</t>
   </si>
 </sst>
 </file>
@@ -353,412 +344,372 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="53">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF9CB9C"/>
-          <bgColor rgb="FFF9CB9C"/>
+  <dxfs count="48">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9CB9C"/>
+          <bgColor rgb="FFF9CB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1091,7 +1042,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1110,10 +1061,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
@@ -1121,7 +1072,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1137,18 +1088,18 @@
         <v>4</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1176,271 +1127,267 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="1"/>
+      <c r="B10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="B11" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
       <c r="C12" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C14" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C16" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
       <c r="C18" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C20" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C22" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="69" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="C24" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C26" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
       <c r="C28" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="69" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
       <c r="C30" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
       <c r="C32" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="69" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D33" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
       <c r="C34" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="69" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="C36" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
       <c r="C38" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="C40" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="C42" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C44" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C46" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1450,46 +1397,26 @@
     </row>
     <row r="49" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C50" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="notContainsBlanks" dxfId="52" priority="52">
+    <cfRule type="notContainsBlanks" dxfId="47" priority="52">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3">
-    <cfRule type="notContainsBlanks" dxfId="50" priority="50">
-      <formula>LEN(TRIM(C3))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4">
-    <cfRule type="notContainsBlanks" dxfId="49" priority="49">
+  <conditionalFormatting sqref="B4:B6">
+    <cfRule type="notContainsBlanks" dxfId="46" priority="47">
       <formula>LEN(TRIM(B4))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5">
-    <cfRule type="notContainsBlanks" dxfId="48" priority="48">
-      <formula>LEN(TRIM(B5))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6">
-    <cfRule type="notContainsBlanks" dxfId="47" priority="47">
-      <formula>LEN(TRIM(B6))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7">
-    <cfRule type="notContainsBlanks" dxfId="46" priority="46">
-      <formula>LEN(TRIM(C7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
@@ -1502,209 +1429,214 @@
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B13">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="42">
+      <formula>LEN(TRIM(B13))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="40">
+      <formula>LEN(TRIM(B15))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="38">
+      <formula>LEN(TRIM(B17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="36">
+      <formula>LEN(TRIM(B19))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="34">
+      <formula>LEN(TRIM(B21))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="32">
+      <formula>LEN(TRIM(B23))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="30">
+      <formula>LEN(TRIM(B25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="28">
+      <formula>LEN(TRIM(B27))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="26">
+      <formula>LEN(TRIM(B29))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31">
+    <cfRule type="notContainsBlanks" dxfId="34" priority="24">
+      <formula>LEN(TRIM(B31))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="22">
+      <formula>LEN(TRIM(B33))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="20">
+      <formula>LEN(TRIM(B35))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="18">
+      <formula>LEN(TRIM(B37))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="16">
+      <formula>LEN(TRIM(B39))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B41">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="14">
+      <formula>LEN(TRIM(B41))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="12">
+      <formula>LEN(TRIM(B43))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="10">
+      <formula>LEN(TRIM(B45))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="8">
+      <formula>LEN(TRIM(B47))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="6">
+      <formula>LEN(TRIM(B49))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="50">
+      <formula>LEN(TRIM(C3))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="46">
+      <formula>LEN(TRIM(C7))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="notContainsBlanks" dxfId="43" priority="43">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="43">
       <formula>LEN(TRIM(C12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13">
-    <cfRule type="notContainsBlanks" dxfId="42" priority="42">
-      <formula>LEN(TRIM(B13))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="notContainsBlanks" dxfId="41" priority="41">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="41">
       <formula>LEN(TRIM(C14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15">
-    <cfRule type="notContainsBlanks" dxfId="40" priority="40">
-      <formula>LEN(TRIM(B15))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="notContainsBlanks" dxfId="39" priority="39">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="39">
       <formula>LEN(TRIM(C16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17">
-    <cfRule type="notContainsBlanks" dxfId="38" priority="38">
-      <formula>LEN(TRIM(B17))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="notContainsBlanks" dxfId="37" priority="37">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="37">
       <formula>LEN(TRIM(C18))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
-    <cfRule type="notContainsBlanks" dxfId="36" priority="36">
-      <formula>LEN(TRIM(B19))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="notContainsBlanks" dxfId="35" priority="35">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="35">
       <formula>LEN(TRIM(C20))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21">
-    <cfRule type="notContainsBlanks" dxfId="34" priority="34">
-      <formula>LEN(TRIM(B21))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="notContainsBlanks" dxfId="33" priority="33">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="33">
       <formula>LEN(TRIM(C22))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B23">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="32">
-      <formula>LEN(TRIM(B23))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="31">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="31">
       <formula>LEN(TRIM(C24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25">
-    <cfRule type="notContainsBlanks" dxfId="30" priority="30">
-      <formula>LEN(TRIM(B25))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="29">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="29">
       <formula>LEN(TRIM(C26))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
-    <cfRule type="notContainsBlanks" dxfId="28" priority="28">
-      <formula>LEN(TRIM(B27))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="notContainsBlanks" dxfId="27" priority="27">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="27">
       <formula>LEN(TRIM(C28))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
-    <cfRule type="notContainsBlanks" dxfId="26" priority="26">
-      <formula>LEN(TRIM(B29))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="notContainsBlanks" dxfId="25" priority="25">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="25">
       <formula>LEN(TRIM(C30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31">
-    <cfRule type="notContainsBlanks" dxfId="24" priority="24">
-      <formula>LEN(TRIM(B31))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="23">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="23">
       <formula>LEN(TRIM(C32))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B33">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="22">
-      <formula>LEN(TRIM(B33))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="21">
       <formula>LEN(TRIM(C34))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B35">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="20">
-      <formula>LEN(TRIM(B35))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="notContainsBlanks" dxfId="19" priority="19">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="19">
       <formula>LEN(TRIM(C36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B37">
-    <cfRule type="notContainsBlanks" dxfId="17" priority="18">
-      <formula>LEN(TRIM(B37))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="notContainsBlanks" dxfId="16" priority="17">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="17">
       <formula>LEN(TRIM(C38))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B39">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="16">
-      <formula>LEN(TRIM(B39))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="15">
       <formula>LEN(TRIM(C40))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B41">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="14">
-      <formula>LEN(TRIM(B41))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="13">
       <formula>LEN(TRIM(C42))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43">
-    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
-      <formula>LEN(TRIM(B43))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="11">
       <formula>LEN(TRIM(C44))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B45">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="10">
-      <formula>LEN(TRIM(B45))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C46">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="9">
       <formula>LEN(TRIM(C46))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B47">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
-      <formula>LEN(TRIM(B47))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="7">
       <formula>LEN(TRIM(C48))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B49">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
-      <formula>LEN(TRIM(B49))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="5">
       <formula>LEN(TRIM(C50))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+  <conditionalFormatting sqref="D4:D5">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(D4))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(D5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">

</xml_diff>